<commit_message>
change id & etc
</commit_message>
<xml_diff>
--- a/storage/excel/test3.xlsx
+++ b/storage/excel/test3.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\daiyas\workspace\daiyas\storage\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB22A700-4224-4D45-B884-773260A10CE8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315EAF0C-2A28-4B5B-8233-1DDE5DF30E17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$3</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,6 +30,34 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>計</t>
+    <rPh sb="0" eb="1">
+      <t>ケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,15 +78,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -63,12 +106,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -84,6 +207,137 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="四角形: 角を丸くする 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A77C4DF-DBC4-4F55-8DFD-21565049D9E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="476250" y="85725"/>
+          <a:ext cx="2476500" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ヘッダ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>214032</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>70037</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>630891</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>155762</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="四角形: 角を丸くする 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{482BF72B-E2A2-48D4-88D0-6586E38D9A78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="897591" y="7779684"/>
+          <a:ext cx="4484594" cy="321049"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>フッタ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,15 +603,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="5" width="17.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" ht="45" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" customHeight="1">
+      <c r="A4" s="1">
+        <f>ROW()-3</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <f>SUM(B4:D4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" customHeight="1">
+      <c r="A5" s="1">
+        <f t="shared" ref="A5:A20" si="0">ROW()-3</f>
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E20" si="1">SUM(B5:D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" customHeight="1">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" customHeight="1">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7:E11" si="2">SUM(B7:D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" customHeight="1">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" customHeight="1">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" customHeight="1">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" customHeight="1">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" customHeight="1">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" customHeight="1">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" customHeight="1">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" customHeight="1">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" customHeight="1">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" customHeight="1">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" customHeight="1">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" customHeight="1">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" customHeight="1" thickBot="1">
+      <c r="A20" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" customHeight="1" thickTop="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7">
+        <f>SUM(E4:E20)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>